<commit_message>
started integrating cometchat for user to user messaging
</commit_message>
<xml_diff>
--- a/business/plan.xlsx
+++ b/business/plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\jbits\Projects\waveybits\devally\business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB298EFA-BA69-4FEB-98A6-2903AD30D9D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54BBDCC-D6BE-471A-A454-705F034DAFB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11865" yWindow="30" windowWidth="34185" windowHeight="20145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12210" yWindow="375" windowWidth="34185" windowHeight="20145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3 Year MRR Projection" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Month #</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>targeted tv ads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post on product hunt </t>
+  </si>
+  <si>
+    <t>Spread in Entrepreneur Magazine</t>
   </si>
 </sst>
 </file>
@@ -948,7 +954,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,6 +1076,9 @@
         <f t="shared" si="1"/>
         <v>1025</v>
       </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
       <c r="I4" t="s">
         <v>8</v>
       </c>
@@ -1350,6 +1359,9 @@
         <f t="shared" si="5"/>
         <v>6725</v>
       </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1453,6 +1465,9 @@
         <f t="shared" si="5"/>
         <v>13025</v>
       </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1503,6 +1518,9 @@
         <f t="shared" si="5"/>
         <v>18150</v>
       </c>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1553,6 +1571,9 @@
         <f t="shared" si="5"/>
         <v>25250</v>
       </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1603,6 +1624,9 @@
         <f t="shared" si="5"/>
         <v>35150</v>
       </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1629,7 +1653,7 @@
         <v>41475</v>
       </c>
       <c r="G25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1681,6 +1705,9 @@
         <f t="shared" si="5"/>
         <v>57800</v>
       </c>
+      <c r="G27" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1807,7 +1834,7 @@
         <v>132275</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1831,8 +1858,11 @@
         <f t="shared" si="5"/>
         <v>156100</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1857,7 +1887,7 @@
         <v>184200</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1882,7 +1912,7 @@
         <v>217350</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1907,7 +1937,7 @@
         <v>256475</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
added meesage box for sending developers a dm
</commit_message>
<xml_diff>
--- a/business/plan.xlsx
+++ b/business/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\jbits\Projects\waveybits\devally\business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54BBDCC-D6BE-471A-A454-705F034DAFB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D66D107-AC7F-4AE5-898D-A5051A2D06CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12210" yWindow="375" windowWidth="34185" windowHeight="20145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Month #</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Spread in Entrepreneur Magazine</t>
+  </si>
+  <si>
+    <t>post on hacker news</t>
   </si>
 </sst>
 </file>
@@ -954,7 +957,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,9 +1113,6 @@
         <f t="shared" si="1"/>
         <v>1350</v>
       </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
       <c r="I5" t="s">
         <v>9</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>1675</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1173,7 +1173,7 @@
         <v>2025</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
         <v>2450</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1229,7 +1229,7 @@
         <v>2925</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1256,6 +1256,9 @@
         <f t="shared" si="5"/>
         <v>3450</v>
       </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1280,6 +1283,9 @@
       <c r="F11" s="3">
         <f t="shared" si="5"/>
         <v>4100</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>